<commit_message>
Added test data files for acceptance testing
</commit_message>
<xml_diff>
--- a/backend/tests/InvalidCourseCatalog.xlsx
+++ b/backend/tests/InvalidCourseCatalog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fruit\sds\2024SpringTeam01-Arts\backend\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabyi\git\2024SpringTeam01-Arts\backend\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3C3B921-C32D-47BE-9586-A61BAD984A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7E7CAF-BCDA-4D02-B0A3-82CABE923C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{EF3B4211-BC02-4438-A3B6-977AC3733487}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15466" xr2:uid="{EF3B4211-BC02-4438-A3B6-977AC3733487}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>CRSE_ID</t>
   </si>
@@ -66,6 +66,21 @@
   </si>
   <si>
     <t>Financial reporting concepts, the accounting information</t>
+  </si>
+  <si>
+    <t>NC_TOPIC</t>
+  </si>
+  <si>
+    <t>instructors</t>
+  </si>
+  <si>
+    <t>email_addresses</t>
+  </si>
+  <si>
+    <t>Dr. Test</t>
+  </si>
+  <si>
+    <t>test@ncsu.edu</t>
   </si>
 </sst>
 </file>
@@ -437,15 +452,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5B0F7A0-5135-49F3-AF70-E17620A2AE76}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,8 +479,23 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>12</v>
       </c>
@@ -483,6 +513,12 @@
       </c>
       <c r="F2" t="s">
         <v>9</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>